<commit_message>
psets: Updated navie-bayes solution in 22
</commit_message>
<xml_diff>
--- a/files/psets/22/Titanic-NaiveBayes-Solution.xlsx
+++ b/files/psets/22/Titanic-NaiveBayes-Solution.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Desktop/NaiveBayes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiverson002\OneDrive - College of Saint Benedict - Saint John's University\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4610F2A3-574B-2F49-B761-0E6705724B8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="6_{A1125C2E-EA3F-4DAC-84F9-4A9D5FF9A494}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{CEB1C759-0C1D-4539-8431-917EF72B8741}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="620" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Titanic" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="12">
   <si>
     <t>male</t>
   </si>
@@ -48,6 +56,15 @@
   <si>
     <t>data probabilities</t>
   </si>
+  <si>
+    <t>P(survive)</t>
+  </si>
+  <si>
+    <t>P(survive|ticket)</t>
+  </si>
+  <si>
+    <t>P(survive|ticket,gender,age)</t>
+  </si>
 </sst>
 </file>
 
@@ -56,7 +73,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -535,17 +552,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -901,18 +921,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>3</v>
       </c>
@@ -929,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3</v>
       </c>
@@ -950,7 +970,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -972,7 +992,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -987,7 +1007,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1003,8 +1023,12 @@
       <c r="G5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1024,10 +1048,29 @@
         <f>COUNTIF($A:$A,H6)/COUNTA($A:$A)</f>
         <v>0.125</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>3</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1047,10 +1090,39 @@
         <f>COUNTIF($A:$A,H7)/COUNTA($A:$A)</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <f>COUNTIFS($D:$D,$K7,$A:$A,L$6)/COUNTIF($A:$A,L$6)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7:N8" si="0">COUNTIFS($D:$D,$K7,$A:$A,M$6)/COUNTIF($A:$A,M$6)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="O7" s="2">
+        <f>COUNTIFS($D:$D,$K7,$B:$B,O$6)/COUNTIF($B:$B,O$6)</f>
+        <v>0.2</v>
+      </c>
+      <c r="P7" s="2">
+        <f>COUNTIFS($D:$D,$K7,$B:$B,P$6)/COUNTIF($B:$B,P$6)</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="Q7" s="2">
+        <f>COUNTIFS($D:$D,$K7,$C:$C,Q$6)/COUNTIF($C:$C,Q$6)</f>
+        <v>0.41176470588235292</v>
+      </c>
+      <c r="R7" s="2">
+        <f>COUNTIFS($D:$D,$K7,$C:$C,R$6)/COUNTIF($C:$C,R$6)</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1071,10 +1143,39 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="J8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <f>COUNTIFS($D:$D,$K8,$A:$A,L$6)/COUNTIF($A:$A,L$6)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="O8" s="2">
+        <f>COUNTIFS($D:$D,$K8,$B:$B,O$6)/COUNTIF($B:$B,O$6)</f>
+        <v>0.8</v>
+      </c>
+      <c r="P8" s="2">
+        <f>COUNTIFS($D:$D,$K8,$B:$B,P$6)/COUNTIF($B:$B,P$6)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="Q8" s="2">
+        <f>COUNTIFS($D:$D,$K8,$C:$C,Q$6)/COUNTIF($C:$C,Q$6)</f>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="R8" s="2">
+        <f>COUNTIFS($D:$D,$K8,$C:$C,R$6)/COUNTIF($C:$C,R$6)</f>
+        <v>0.8571428571428571</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1094,10 +1195,11 @@
         <f>COUNTIF($B:$B,H9)/COUNTA($B:$B)</f>
         <v>0.625</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1118,10 +1220,11 @@
         <v>0.375</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1141,10 +1244,11 @@
         <f>COUNTIF($C:$C,H11)/COUNTA($C:$C)</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K11" s="1"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1165,10 +1269,11 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="J12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K12" s="1"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1181,8 +1286,11 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1200,7 +1308,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1220,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1237,16 +1345,16 @@
         <v>1</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" ref="H16:I18" si="0">COUNTIFS($A:$A,$G16,$D:$D,H$15)/COUNTIF($D:$D,H$15)</f>
+        <f t="shared" ref="H16:I18" si="1">COUNTIFS($A:$A,$G16,$D:$D,H$15)/COUNTIF($D:$D,H$15)</f>
         <v>0.125</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1263,15 +1371,15 @@
         <v>2</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.625</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1288,17 +1396,17 @@
         <v>3</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1323,7 +1431,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1350,7 +1458,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1375,7 +1483,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1402,7 +1510,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1419,7 +1527,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1432,56 +1540,96 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4" t="s">
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="4"/>
+      <c r="K24" s="6"/>
       <c r="L24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="3">
+        <f>I2</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K27" s="3">
+        <f>I3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L27">
+        <f>IF(J27&gt;K27,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="3">
+        <f>HLOOKUP($G$25,$L$6:$N$8,2)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K28" s="3">
+        <f>HLOOKUP($G$25,$L$6:$N$8,3)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L28">
+        <f>IF(J28&gt;K28,0,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="3">
         <f>VLOOKUP($G$25,$G$16:$I$18,2)*VLOOKUP($H$25,$G$19:$I$20,2)*VLOOKUP($I$25,$G$21:$I$22,2)*$I$2</f>
-        <v>9.5703125E-2</v>
-      </c>
-      <c r="K25" s="5">
+        <v>2.2786458333333332E-2</v>
+      </c>
+      <c r="K29" s="3">
         <f>VLOOKUP($G$25,$G$16:$I$18,3)*VLOOKUP($H$25,$G$19:$I$20,3)*VLOOKUP($I$25,$G$21:$I$22,3)*$I$3</f>
-        <v>7.8125E-2</v>
-      </c>
-      <c r="L25">
-        <f>IF(J25&gt;K25,0,1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J27">
-        <f>VLOOKUP($G$25,$G$16:$I$18,2)*$I$2</f>
-        <v>0.29166666666666663</v>
-      </c>
-      <c r="K27">
-        <f>VLOOKUP($G$25,$G$16:$I$18,3)*$I$3</f>
-        <v>0.16666666666666666</v>
+        <v>1.3020833333333332E-2</v>
+      </c>
+      <c r="L29">
+        <f>IF(J29&gt;K29,0,1)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="J24:K24"/>
+    <mergeCell ref="G27:I27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>